<commit_message>
Adds updated adjacency excel spreadsheet
</commit_message>
<xml_diff>
--- a/docs/DistrictAdjacencies.xlsx
+++ b/docs/DistrictAdjacencies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/594db1e7acc97ba9/Documents/GitHub/Civ-VII-District-Mod/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5393AD1E-3BC6-47E1-B71D-2A56BF43A1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{5393AD1E-3BC6-47E1-B71D-2A56BF43A1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{802E4C38-6903-4896-A63D-24552AF5F662}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="18000" windowHeight="11170" xr2:uid="{1AAE061A-9CCE-4CFD-9D60-99C8FE53EF84}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{1AAE061A-9CCE-4CFD-9D60-99C8FE53EF84}"/>
   </bookViews>
   <sheets>
     <sheet name="DistrictAdjaceny" sheetId="1" r:id="rId1"/>
@@ -36,25 +36,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>District</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Requirement</t>
   </si>
   <si>
     <t>Adjacency Bonus</t>
+  </si>
+  <si>
+    <t>Civ VII</t>
+  </si>
+  <si>
+    <t>Civ VI</t>
+  </si>
+  <si>
+    <t>Campus</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Science from Mountains + 1</t>
+  </si>
+  <si>
+    <t>Science from Reef +1</t>
+  </si>
+  <si>
+    <t>Science from Mountains +1</t>
+  </si>
+  <si>
+    <t>Science from Jungle +1</t>
+  </si>
+  <si>
+    <t>Ageless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library + Garden </t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>https://civilization.fandom.com/wiki/List_of_quarters_in_Civ7</t>
+  </si>
+  <si>
+    <t>Built out urban quarters gives +1 science</t>
+  </si>
+  <si>
+    <t>Scholarium Quarter</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Astronomer Quarter</t>
+  </si>
+  <si>
+    <t>Library + 3 Mountains</t>
+  </si>
+  <si>
+    <t>European/Asian/America</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,13 +136,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,23 +478,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621453A8-86D6-48DB-81C2-E2540C577F62}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" customWidth="1"/>
+    <col min="5" max="5" width="32.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>